<commit_message>
Validating expected outcome from Excel sheet data, completed
</commit_message>
<xml_diff>
--- a/MyJava/src/ArrowMiiData/ArrowMiiTestData.xlsx
+++ b/MyJava/src/ArrowMiiData/ArrowMiiTestData.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="3680" windowWidth="27760" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="27760" windowHeight="15300" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario2" sheetId="2" r:id="rId2"/>
+    <sheet name="Scenario3" sheetId="4" r:id="rId3"/>
+    <sheet name="Scenario4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>TestCase ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Groups To Trigger values</t>
   </si>
@@ -85,10 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,85 +368,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8">
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="B8" s="4">
         <v>12</v>
       </c>
     </row>

</xml_diff>